<commit_message>
Burndown charts for Sprint 1 & 2
</commit_message>
<xml_diff>
--- a/Diagrams/Sprint 1/Burnout Chart Sprint 1.xlsx
+++ b/Diagrams/Sprint 1/Burnout Chart Sprint 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\StockManager-master\Diagrams\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -134,7 +134,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -147,6 +147,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -389,45 +392,69 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'MANUFACTURING OUTPUT'!$B$4:$B$27</c:f>
+              <c:f>'MANUFACTURING OUTPUT'!$B$4:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>43025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43026</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43027</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43028</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43029</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43030</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>43031</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="7">
                   <c:v>43032</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
                   <c:v>43033</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>43034</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
                   <c:v>43035</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11">
                   <c:v>43036</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12">
                   <c:v>43037</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43038</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43039</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'MANUFACTURING OUTPUT'!$C$4:$C$27</c:f>
+              <c:f>'MANUFACTURING OUTPUT'!$C$4:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -442,6 +469,30 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -463,11 +514,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="41"/>
-        <c:axId val="310910968"/>
-        <c:axId val="310906264"/>
+        <c:axId val="300934360"/>
+        <c:axId val="300926912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="310910968"/>
+        <c:axId val="300934360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +556,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310906264"/>
+        <c:crossAx val="300926912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -513,7 +564,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="310906264"/>
+        <c:axId val="300926912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -523,7 +574,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="310910968"/>
+        <c:crossAx val="300934360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1179,7 +1230,7 @@
         <xdr:cNvPr id="2" name="Chart 1" descr="Column chart showing date and number of components completed. Sort the Date column to see dates in Ascending or Descending order">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1203,8 +1254,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Data" displayName="Data" ref="B3:C27" totalsRowShown="0" headerRowCellStyle="Heading 1">
-  <autoFilter ref="B3:C27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Data" displayName="Data" ref="B3:C35" totalsRowShown="0" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B3:C35">
     <filterColumn colId="1">
       <filters>
         <filter val="0"/>
@@ -1458,10 +1509,10 @@
     <tabColor theme="5"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:C27"/>
+  <dimension ref="B1:C35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,7 +1543,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
-        <v>43031</v>
+        <v>43025</v>
       </c>
       <c r="C4" s="5">
         <v>2</v>
@@ -1501,16 +1552,16 @@
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
-        <v>43032</v>
+        <v>43026</v>
       </c>
       <c r="C5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <f t="shared" ref="B6:B10" ca="1" si="0">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
-        <v>43033</v>
+        <v>43027</v>
       </c>
       <c r="C6" s="5">
         <v>0</v>
@@ -1519,7 +1570,7 @@
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>43034</v>
+        <v>43028</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -1528,7 +1579,7 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>43035</v>
+        <v>43029</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -1537,7 +1588,7 @@
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>43036</v>
+        <v>43030</v>
       </c>
       <c r="C9" s="5">
         <v>0</v>
@@ -1546,7 +1597,7 @@
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>43037</v>
+        <v>43031</v>
       </c>
       <c r="C10" s="5">
         <v>0</v>
@@ -1555,7 +1606,7 @@
     <row r="11" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <f ca="1">TODAY()+7</f>
-        <v>43046</v>
+        <v>43067</v>
       </c>
       <c r="C11" s="5">
         <v>25</v>
@@ -1564,7 +1615,7 @@
     <row r="12" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <f ca="1">TODAY()+8</f>
-        <v>43047</v>
+        <v>43068</v>
       </c>
       <c r="C12" s="5">
         <v>73</v>
@@ -1573,7 +1624,7 @@
     <row r="13" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <f ca="1">TODAY()+9</f>
-        <v>43048</v>
+        <v>43069</v>
       </c>
       <c r="C13" s="5">
         <v>40</v>
@@ -1582,7 +1633,7 @@
     <row r="14" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <f ca="1">TODAY()+10</f>
-        <v>43049</v>
+        <v>43070</v>
       </c>
       <c r="C14" s="5">
         <v>57</v>
@@ -1591,7 +1642,7 @@
     <row r="15" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <f ca="1">TODAY()+11</f>
-        <v>43050</v>
+        <v>43071</v>
       </c>
       <c r="C15" s="5">
         <v>64</v>
@@ -1600,7 +1651,7 @@
     <row r="16" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <f ca="1">TODAY()+12</f>
-        <v>43051</v>
+        <v>43072</v>
       </c>
       <c r="C16" s="5">
         <v>48</v>
@@ -1609,7 +1660,7 @@
     <row r="17" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <f ca="1">TODAY()+13</f>
-        <v>43052</v>
+        <v>43073</v>
       </c>
       <c r="C17" s="5">
         <v>54</v>
@@ -1618,7 +1669,7 @@
     <row r="18" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <f ca="1">TODAY()+14</f>
-        <v>43053</v>
+        <v>43074</v>
       </c>
       <c r="C18" s="5">
         <v>42</v>
@@ -1627,7 +1678,7 @@
     <row r="19" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <f ca="1">TODAY()+15</f>
-        <v>43054</v>
+        <v>43075</v>
       </c>
       <c r="C19" s="5">
         <v>31</v>
@@ -1636,7 +1687,7 @@
     <row r="20" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <f ca="1">TODAY()+16</f>
-        <v>43055</v>
+        <v>43076</v>
       </c>
       <c r="C20" s="5">
         <v>62</v>
@@ -1645,7 +1696,7 @@
     <row r="21" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <f ca="1">TODAY()+17</f>
-        <v>43056</v>
+        <v>43077</v>
       </c>
       <c r="C21" s="5">
         <v>53</v>
@@ -1654,7 +1705,7 @@
     <row r="22" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <f ca="1">TODAY()+18</f>
-        <v>43057</v>
+        <v>43078</v>
       </c>
       <c r="C22" s="5">
         <v>72</v>
@@ -1663,7 +1714,7 @@
     <row r="23" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <f ca="1">TODAY()+19</f>
-        <v>43058</v>
+        <v>43079</v>
       </c>
       <c r="C23" s="5">
         <v>69</v>
@@ -1672,7 +1723,7 @@
     <row r="24" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <f ca="1">TODAY()+20</f>
-        <v>43059</v>
+        <v>43080</v>
       </c>
       <c r="C24" s="5">
         <v>58</v>
@@ -1681,7 +1732,7 @@
     <row r="25" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <f ca="1">TODAY()+21</f>
-        <v>43060</v>
+        <v>43081</v>
       </c>
       <c r="C25" s="5">
         <v>71</v>
@@ -1690,7 +1741,7 @@
     <row r="26" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <f ca="1">TODAY()+22</f>
-        <v>43061</v>
+        <v>43082</v>
       </c>
       <c r="C26" s="5">
         <v>60</v>
@@ -1699,10 +1750,80 @@
     <row r="27" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <f ca="1">TODAY()+23</f>
-        <v>43062</v>
+        <v>43083</v>
       </c>
       <c r="C27" s="5">
         <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <v>43032</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <v>43033</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <v>43034</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <v>43035</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
+        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <v>43036</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <v>43037</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
+        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <v>43038</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
+        <v>43039</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Editted burnout chart to account for unrecorded time.
</commit_message>
<xml_diff>
--- a/Diagrams/Sprint 1/Burnout Chart Sprint 1.xlsx
+++ b/Diagrams/Sprint 1/Burnout Chart Sprint 1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\StockManager-master\Diagrams\Sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\StockManager\Diagrams\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="MANUFACTURING OUTPUT" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="ColumnTitle1">Data[[#Headers],[Date]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'MANUFACTURING OUTPUT'!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -257,7 +257,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -370,9 +369,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -472,7 +470,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
                   <c:v>1</c:v>
@@ -498,7 +496,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-01AB-496F-ACDD-F58747B8C0B7}"/>
             </c:ext>
@@ -1230,7 +1228,7 @@
         <xdr:cNvPr id="2" name="Chart 1" descr="Column chart showing date and number of components completed. Sort the Date column to see dates in Ascending or Descending order">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1512,7 +1510,7 @@
   <dimension ref="B1:C35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1604,7 @@
     <row r="11" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <f ca="1">TODAY()+7</f>
-        <v>43067</v>
+        <v>43078</v>
       </c>
       <c r="C11" s="5">
         <v>25</v>
@@ -1615,7 +1613,7 @@
     <row r="12" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <f ca="1">TODAY()+8</f>
-        <v>43068</v>
+        <v>43079</v>
       </c>
       <c r="C12" s="5">
         <v>73</v>
@@ -1624,7 +1622,7 @@
     <row r="13" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <f ca="1">TODAY()+9</f>
-        <v>43069</v>
+        <v>43080</v>
       </c>
       <c r="C13" s="5">
         <v>40</v>
@@ -1633,7 +1631,7 @@
     <row r="14" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <f ca="1">TODAY()+10</f>
-        <v>43070</v>
+        <v>43081</v>
       </c>
       <c r="C14" s="5">
         <v>57</v>
@@ -1642,7 +1640,7 @@
     <row r="15" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <f ca="1">TODAY()+11</f>
-        <v>43071</v>
+        <v>43082</v>
       </c>
       <c r="C15" s="5">
         <v>64</v>
@@ -1651,7 +1649,7 @@
     <row r="16" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <f ca="1">TODAY()+12</f>
-        <v>43072</v>
+        <v>43083</v>
       </c>
       <c r="C16" s="5">
         <v>48</v>
@@ -1660,7 +1658,7 @@
     <row r="17" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <f ca="1">TODAY()+13</f>
-        <v>43073</v>
+        <v>43084</v>
       </c>
       <c r="C17" s="5">
         <v>54</v>
@@ -1669,7 +1667,7 @@
     <row r="18" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <f ca="1">TODAY()+14</f>
-        <v>43074</v>
+        <v>43085</v>
       </c>
       <c r="C18" s="5">
         <v>42</v>
@@ -1678,7 +1676,7 @@
     <row r="19" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <f ca="1">TODAY()+15</f>
-        <v>43075</v>
+        <v>43086</v>
       </c>
       <c r="C19" s="5">
         <v>31</v>
@@ -1687,7 +1685,7 @@
     <row r="20" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <f ca="1">TODAY()+16</f>
-        <v>43076</v>
+        <v>43087</v>
       </c>
       <c r="C20" s="5">
         <v>62</v>
@@ -1696,7 +1694,7 @@
     <row r="21" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <f ca="1">TODAY()+17</f>
-        <v>43077</v>
+        <v>43088</v>
       </c>
       <c r="C21" s="5">
         <v>53</v>
@@ -1705,7 +1703,7 @@
     <row r="22" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <f ca="1">TODAY()+18</f>
-        <v>43078</v>
+        <v>43089</v>
       </c>
       <c r="C22" s="5">
         <v>72</v>
@@ -1714,7 +1712,7 @@
     <row r="23" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <f ca="1">TODAY()+19</f>
-        <v>43079</v>
+        <v>43090</v>
       </c>
       <c r="C23" s="5">
         <v>69</v>
@@ -1723,7 +1721,7 @@
     <row r="24" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <f ca="1">TODAY()+20</f>
-        <v>43080</v>
+        <v>43091</v>
       </c>
       <c r="C24" s="5">
         <v>58</v>
@@ -1732,7 +1730,7 @@
     <row r="25" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <f ca="1">TODAY()+21</f>
-        <v>43081</v>
+        <v>43092</v>
       </c>
       <c r="C25" s="5">
         <v>71</v>
@@ -1741,7 +1739,7 @@
     <row r="26" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <f ca="1">TODAY()+22</f>
-        <v>43082</v>
+        <v>43093</v>
       </c>
       <c r="C26" s="5">
         <v>60</v>
@@ -1750,7 +1748,7 @@
     <row r="27" spans="2:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <f ca="1">TODAY()+23</f>
-        <v>43083</v>
+        <v>43094</v>
       </c>
       <c r="C27" s="5">
         <v>64</v>
@@ -1761,12 +1759,12 @@
         <v>43032</v>
       </c>
       <c r="C28" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="6">
-        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <f t="shared" ref="B29:B34" ca="1" si="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
         <v>43033</v>
       </c>
       <c r="C29" s="3">
@@ -1775,7 +1773,7 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="6">
-        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <f t="shared" ca="1" si="1"/>
         <v>43034</v>
       </c>
       <c r="C30" s="3">
@@ -1784,7 +1782,7 @@
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
-        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <f t="shared" ca="1" si="1"/>
         <v>43035</v>
       </c>
       <c r="C31" s="3">
@@ -1793,7 +1791,7 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
-        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <f t="shared" ca="1" si="1"/>
         <v>43036</v>
       </c>
       <c r="C32" s="3">
@@ -1802,7 +1800,7 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="6">
-        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <f t="shared" ca="1" si="1"/>
         <v>43037</v>
       </c>
       <c r="C33" s="3">
@@ -1811,7 +1809,7 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="6">
-        <f ca="1">INDIRECT(ADDRESS(ROW()-1,COLUMN()))+1</f>
+        <f t="shared" ca="1" si="1"/>
         <v>43038</v>
       </c>
       <c r="C34" s="3">

</xml_diff>